<commit_message>
add skates into quota/catch, sep groundfish and small mesh
</commit_message>
<xml_diff>
--- a/data-raw/NEFMC_abc_acl.xlsx
+++ b/data-raw/NEFMC_abc_acl.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2241" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2292" uniqueCount="97">
   <si>
     <t>Time</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>Initial Value in million lb converted using =(Value*1000000)/2205</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Skates (Wings)*</t>
+  </si>
+  <si>
+    <t>Skate*</t>
   </si>
 </sst>
 </file>
@@ -1698,8 +1707,8 @@
   <dimension ref="A1:I293"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A252" sqref="A252:F261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8198,10 +8207,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O329"/>
+  <dimension ref="A1:O344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="D334" sqref="D334"/>
+    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="D330" sqref="D330:D339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16771,7 +16780,7 @@
         <v>2018</v>
       </c>
       <c r="D324" s="137">
-        <f t="shared" ref="D323:E329" si="5">(K324*1000000)/2205</f>
+        <f t="shared" ref="D324:E329" si="5">(K324*1000000)/2205</f>
         <v>22630.385487528343</v>
       </c>
       <c r="E324" s="137">
@@ -16785,7 +16794,7 @@
         <v>56</v>
       </c>
       <c r="H324" s="137">
-        <f t="shared" ref="F322:H329" si="6">(O324*1000000)/2205</f>
+        <f t="shared" ref="H324:H329" si="6">(O324*1000000)/2205</f>
         <v>11569.160997732426</v>
       </c>
       <c r="K324" s="126">
@@ -17022,6 +17031,272 @@
       </c>
       <c r="O329" s="138">
         <v>28.5</v>
+      </c>
+    </row>
+    <row r="330" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A330" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B330" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C330" s="12">
+        <v>2022</v>
+      </c>
+      <c r="D330" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E330" s="12">
+        <v>2947</v>
+      </c>
+      <c r="F330" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G330" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="H330" s="12">
+        <v>14059.1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A331" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="B331" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C331" s="12">
+        <v>2021</v>
+      </c>
+      <c r="D331" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E331" s="12">
+        <v>4793</v>
+      </c>
+      <c r="F331" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G331" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="H331" s="12">
+        <v>11879</v>
+      </c>
+    </row>
+    <row r="332" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A332" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="B332" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C332" s="12">
+        <v>2020</v>
+      </c>
+      <c r="D332" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E332" s="12">
+        <v>9158</v>
+      </c>
+      <c r="F332" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G332" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="H332" s="12">
+        <v>11879</v>
+      </c>
+    </row>
+    <row r="333" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A333" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="B333" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C333" s="12">
+        <v>2019</v>
+      </c>
+      <c r="D333" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E333" s="12">
+        <v>8494.7999999999993</v>
+      </c>
+      <c r="F333" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G333" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="H333" s="12">
+        <v>10499</v>
+      </c>
+    </row>
+    <row r="334" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A334" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="B334" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C334" s="12">
+        <v>2018</v>
+      </c>
+      <c r="D334" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E334" s="12">
+        <v>9223.5</v>
+      </c>
+      <c r="F334" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G334" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="H334" s="12">
+        <v>10499</v>
+      </c>
+    </row>
+    <row r="335" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A335" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="B335" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C335" s="12">
+        <v>2017</v>
+      </c>
+      <c r="D335" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E335" s="12">
+        <v>8426.4</v>
+      </c>
+      <c r="F335" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G335" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="H335" s="12">
+        <v>8372</v>
+      </c>
+    </row>
+    <row r="336" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A336" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="B336" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C336" s="12">
+        <v>2016</v>
+      </c>
+      <c r="D336" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E336" s="12">
+        <v>8190.7</v>
+      </c>
+      <c r="F336" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G336" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="H336" s="12">
+        <v>8372</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A337" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="B337" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C337" s="12">
+        <v>2015</v>
+      </c>
+      <c r="D337" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E337" s="12">
+        <v>8647.9</v>
+      </c>
+      <c r="F337" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G337" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="H337" s="12">
+        <v>10896.2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A338" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="B338" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C338" s="12">
+        <v>2014</v>
+      </c>
+      <c r="D338" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E338" s="12">
+        <v>10232.299999999999</v>
+      </c>
+      <c r="F338" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G338" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="H338" s="12">
+        <v>10896.2</v>
+      </c>
+    </row>
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A339" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="B339" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C339" s="12">
+        <v>2013</v>
+      </c>
+      <c r="D339" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E339" s="12">
+        <v>7988.4</v>
+      </c>
+      <c r="F339" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G339" s="137" t="s">
+        <v>56</v>
+      </c>
+      <c r="H339" s="12">
+        <v>14338</v>
+      </c>
+    </row>
+    <row r="342" spans="1:8" s="137" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E344" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>